<commit_message>
Update manual error sampling.
Updated manual error analysis sampling to make error categories mutually
exclusive. Updated final reason category to be more descriptive and
reduced the total number of categories.
</commit_message>
<xml_diff>
--- a/crowd_only/data/final_eval/analysis/crowd_testset_perfect_ner_errors.xlsx
+++ b/crowd_only/data/final_eval/analysis/crowd_testset_perfect_ner_errors.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="345">
   <si>
     <t>pmid</t>
   </si>
@@ -371,7 +371,7 @@
     <t>https://crowdflower.com/jobs/767262/units/773932578</t>
   </si>
   <si>
-    <t>gold_error</t>
+    <t>missing_relation</t>
   </si>
   <si>
     <t>Trimethaphan caused different results depending on which rat type it was. I think the gold went with tachycardia because the sham rats were not given the lesion?</t>
@@ -401,10 +401,7 @@
     <t>https://crowdflower.com/jobs/767262/units/773932960</t>
   </si>
   <si>
-    <t>ambiguous</t>
-  </si>
-  <si>
-    <t>Disagreement with the gold arises from whether “hypersensitivity” is different from “hypersensiitivity to sodium pentobarbital. Also gold used barium chloride, when ostensibly the chloride is just a way to deliver barium.</t>
+    <t>Disagreement with the gold arises from whether “hypersensitivity” is different from “hypersensitivity to sodium pentobarbital. Also gold used barium chloride, when ostensibly the chloride is just a way to deliver barium.</t>
   </si>
   <si>
     <t>https://crowdflower.com/jobs/767262/units/773932961</t>
@@ -458,9 +455,6 @@
     <t>https://crowdflower.com/jobs/767262/units/773933843</t>
   </si>
   <si>
-    <t>gold_inconsistent</t>
-  </si>
-  <si>
     <t>Gold is inconsistent with how it treats chemical disease statements.</t>
   </si>
   <si>
@@ -488,9 +482,6 @@
     <t>https://crowdflower.com/jobs/767262/units/773931741</t>
   </si>
   <si>
-    <t>ner_error</t>
-  </si>
-  <si>
     <t>Rapamycin is highlighted as a chemical, but in context the real concept is mTOR inhibitors. We have seen that the crowd is terrible at recognizing bad NER.</t>
   </si>
   <si>
@@ -755,6 +746,9 @@
     <t>https://crowdflower.com/jobs/767262/units/773932434</t>
   </si>
   <si>
+    <t>false_relation</t>
+  </si>
+  <si>
     <t>Text never says that EACA causes SAH. If anything, it only says that EACA is good for treating rebleeding for patients with SAH.</t>
   </si>
   <si>
@@ -963,9 +957,6 @@
   </si>
   <si>
     <t>https://crowdflower.com/jobs/767273/units/773937562</t>
-  </si>
-  <si>
-    <t>implicit_relation</t>
   </si>
   <si>
     <t>Text states that rate of a disease is same between two groups treated with a drug. This does not necessarily mean that the drug causes the disease, but does imply it. Grey area in my opinion.</t>
@@ -1189,8 +1180,8 @@
   </sheetPr>
   <dimension ref="A1:L122"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A21" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L47" activeCellId="0" sqref="L47"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A85" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K105" activeCellId="0" sqref="K105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2356,7 +2347,7 @@
         <v>1</v>
       </c>
       <c r="I48" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J48" s="0" t="n">
         <v>0</v>
@@ -2368,7 +2359,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="n">
         <v>3975902</v>
       </c>
@@ -2400,10 +2391,10 @@
         <v>0</v>
       </c>
       <c r="K49" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="L49" s="0" t="s">
         <v>128</v>
-      </c>
-      <c r="L49" s="0" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2423,7 +2414,7 @@
         <v>4</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G50" s="0" t="s">
         <v>114</v>
@@ -2438,10 +2429,10 @@
         <v>0</v>
       </c>
       <c r="K50" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="L50" s="0" t="s">
         <v>128</v>
-      </c>
-      <c r="L50" s="0" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2449,10 +2440,10 @@
         <v>3987172</v>
       </c>
       <c r="B51" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="C51" s="0" t="s">
         <v>131</v>
-      </c>
-      <c r="C51" s="0" t="s">
-        <v>132</v>
       </c>
       <c r="D51" s="0" t="s">
         <v>14</v>
@@ -2461,7 +2452,7 @@
         <v>5</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G51" s="0" t="s">
         <v>114</v>
@@ -2479,7 +2470,7 @@
         <v>118</v>
       </c>
       <c r="L51" s="0" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2487,10 +2478,10 @@
         <v>3990093</v>
       </c>
       <c r="B52" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="C52" s="0" t="s">
         <v>135</v>
-      </c>
-      <c r="C52" s="0" t="s">
-        <v>136</v>
       </c>
       <c r="D52" s="0" t="s">
         <v>14</v>
@@ -2499,7 +2490,7 @@
         <v>4</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G52" s="0" t="s">
         <v>114</v>
@@ -2517,7 +2508,7 @@
         <v>123</v>
       </c>
       <c r="L52" s="0" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2525,10 +2516,10 @@
         <v>3990093</v>
       </c>
       <c r="B53" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="C53" s="0" t="s">
         <v>135</v>
-      </c>
-      <c r="C53" s="0" t="s">
-        <v>136</v>
       </c>
       <c r="D53" s="0" t="s">
         <v>14</v>
@@ -2537,7 +2528,7 @@
         <v>4</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G53" s="0" t="s">
         <v>114</v>
@@ -2555,7 +2546,7 @@
         <v>123</v>
       </c>
       <c r="L53" s="0" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2563,10 +2554,10 @@
         <v>10939760</v>
       </c>
       <c r="B54" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="C54" s="0" t="s">
         <v>140</v>
-      </c>
-      <c r="C54" s="0" t="s">
-        <v>141</v>
       </c>
       <c r="D54" s="0" t="s">
         <v>14</v>
@@ -2575,7 +2566,7 @@
         <v>5</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G54" s="0" t="s">
         <v>114</v>
@@ -2593,18 +2584,18 @@
         <v>118</v>
       </c>
       <c r="L54" s="0" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="n">
         <v>12828076</v>
       </c>
       <c r="B55" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="C55" s="0" t="s">
         <v>144</v>
-      </c>
-      <c r="C55" s="0" t="s">
-        <v>145</v>
       </c>
       <c r="D55" s="0" t="s">
         <v>14</v>
@@ -2613,7 +2604,7 @@
         <v>4</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G55" s="0" t="s">
         <v>114</v>
@@ -2628,10 +2619,10 @@
         <v>0</v>
       </c>
       <c r="K55" s="0" t="s">
-        <v>147</v>
+        <v>123</v>
       </c>
       <c r="L55" s="0" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2639,10 +2630,10 @@
         <v>12828076</v>
       </c>
       <c r="B56" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="C56" s="0" t="s">
         <v>144</v>
-      </c>
-      <c r="C56" s="0" t="s">
-        <v>145</v>
       </c>
       <c r="D56" s="0" t="s">
         <v>14</v>
@@ -2651,7 +2642,7 @@
         <v>4</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G56" s="0" t="s">
         <v>114</v>
@@ -2666,13 +2657,13 @@
         <v>0</v>
       </c>
       <c r="K56" s="0" t="s">
-        <v>147</v>
+        <v>123</v>
       </c>
       <c r="L56" s="0" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="n">
         <v>18801087</v>
       </c>
@@ -2689,7 +2680,7 @@
         <v>5</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G57" s="0" t="s">
         <v>114</v>
@@ -2707,18 +2698,18 @@
         <v>118</v>
       </c>
       <c r="L57" s="0" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="n">
         <v>22836123</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D58" s="0" t="s">
         <v>14</v>
@@ -2727,7 +2718,7 @@
         <v>5</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G58" s="0" t="s">
         <v>114</v>
@@ -2745,10 +2736,10 @@
         <v>118</v>
       </c>
       <c r="L58" s="0" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="n">
         <v>24040781</v>
       </c>
@@ -2765,7 +2756,7 @@
         <v>4</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G59" s="0" t="s">
         <v>114</v>
@@ -2774,16 +2765,16 @@
         <v>1</v>
       </c>
       <c r="I59" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J59" s="0" t="n">
         <v>0</v>
       </c>
       <c r="K59" s="0" t="s">
-        <v>157</v>
+        <v>123</v>
       </c>
       <c r="L59" s="0" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2794,7 +2785,7 @@
         <v>50</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D60" s="0" t="s">
         <v>14</v>
@@ -2803,7 +2794,7 @@
         <v>4</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="G60" s="0" t="s">
         <v>114</v>
@@ -2821,7 +2812,7 @@
         <v>118</v>
       </c>
       <c r="L60" s="0" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2829,10 +2820,10 @@
         <v>24209900</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D61" s="0" t="s">
         <v>14</v>
@@ -2841,7 +2832,7 @@
         <v>5</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="G61" s="0" t="s">
         <v>114</v>
@@ -2850,16 +2841,16 @@
         <v>0</v>
       </c>
       <c r="I61" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J61" s="0" t="n">
         <v>0</v>
       </c>
       <c r="K61" s="0" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="L61" s="0" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2867,10 +2858,10 @@
         <v>24209900</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D62" s="0" t="s">
         <v>14</v>
@@ -2879,7 +2870,7 @@
         <v>5</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="G62" s="0" t="s">
         <v>114</v>
@@ -2888,16 +2879,16 @@
         <v>0</v>
       </c>
       <c r="I62" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J62" s="0" t="n">
         <v>0</v>
       </c>
       <c r="K62" s="0" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="L62" s="0" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2905,10 +2896,10 @@
         <v>24209900</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D63" s="0" t="s">
         <v>14</v>
@@ -2917,7 +2908,7 @@
         <v>5</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="G63" s="0" t="s">
         <v>114</v>
@@ -2926,16 +2917,16 @@
         <v>0</v>
       </c>
       <c r="I63" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J63" s="0" t="n">
         <v>0</v>
       </c>
       <c r="K63" s="0" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="L63" s="0" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2943,10 +2934,10 @@
         <v>24209900</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D64" s="0" t="s">
         <v>14</v>
@@ -2955,7 +2946,7 @@
         <v>5</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="G64" s="0" t="s">
         <v>114</v>
@@ -2964,16 +2955,16 @@
         <v>0</v>
       </c>
       <c r="I64" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J64" s="0" t="n">
         <v>0</v>
       </c>
       <c r="K64" s="0" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="L64" s="0" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2981,10 +2972,10 @@
         <v>24209900</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D65" s="0" t="s">
         <v>14</v>
@@ -2993,7 +2984,7 @@
         <v>5</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="G65" s="0" t="s">
         <v>114</v>
@@ -3002,16 +2993,16 @@
         <v>0</v>
       </c>
       <c r="I65" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J65" s="0" t="n">
         <v>0</v>
       </c>
       <c r="K65" s="0" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="L65" s="0" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3019,10 +3010,10 @@
         <v>24209900</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D66" s="0" t="s">
         <v>14</v>
@@ -3031,7 +3022,7 @@
         <v>5</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="G66" s="0" t="s">
         <v>114</v>
@@ -3040,27 +3031,27 @@
         <v>0</v>
       </c>
       <c r="I66" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J66" s="0" t="n">
         <v>0</v>
       </c>
       <c r="K66" s="0" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="L66" s="0" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="n">
         <v>24209900</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D67" s="0" t="s">
         <v>14</v>
@@ -3069,7 +3060,7 @@
         <v>5</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="G67" s="0" t="s">
         <v>114</v>
@@ -3078,27 +3069,27 @@
         <v>0</v>
       </c>
       <c r="I67" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J67" s="0" t="n">
         <v>0</v>
       </c>
       <c r="K67" s="0" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="L67" s="0" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="n">
         <v>24840785</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D68" s="0" t="s">
         <v>14</v>
@@ -3107,7 +3098,7 @@
         <v>4</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="G68" s="0" t="s">
         <v>114</v>
@@ -3125,7 +3116,7 @@
         <v>118</v>
       </c>
       <c r="L68" s="0" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3133,10 +3124,10 @@
         <v>24840785</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D69" s="0" t="s">
         <v>14</v>
@@ -3145,7 +3136,7 @@
         <v>4</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="G69" s="0" t="s">
         <v>114</v>
@@ -3163,7 +3154,7 @@
         <v>118</v>
       </c>
       <c r="L69" s="0" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3171,10 +3162,10 @@
         <v>25071004</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D70" s="0" t="s">
         <v>14</v>
@@ -3183,7 +3174,7 @@
         <v>4</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="G70" s="0" t="s">
         <v>114</v>
@@ -3192,27 +3183,27 @@
         <v>0</v>
       </c>
       <c r="I70" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J70" s="0" t="n">
         <v>0</v>
       </c>
       <c r="K70" s="0" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="L70" s="0" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="n">
         <v>733189</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D71" s="0" t="s">
         <v>74</v>
@@ -3221,7 +3212,7 @@
         <v>5</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="G71" s="0" t="s">
         <v>114</v>
@@ -3239,18 +3230,18 @@
         <v>118</v>
       </c>
       <c r="L71" s="0" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="n">
         <v>733189</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D72" s="0" t="s">
         <v>74</v>
@@ -3259,7 +3250,7 @@
         <v>5</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="G72" s="0" t="s">
         <v>114</v>
@@ -3277,10 +3268,10 @@
         <v>118</v>
       </c>
       <c r="L72" s="0" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="n">
         <v>3289726</v>
       </c>
@@ -3288,7 +3279,7 @@
         <v>82</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D73" s="0" t="s">
         <v>74</v>
@@ -3297,7 +3288,7 @@
         <v>5</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="G73" s="0" t="s">
         <v>114</v>
@@ -3315,15 +3306,15 @@
         <v>118</v>
       </c>
       <c r="L73" s="0" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="n">
         <v>3323259</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C74" s="0" t="s">
         <v>100</v>
@@ -3335,7 +3326,7 @@
         <v>4</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G74" s="0" t="s">
         <v>114</v>
@@ -3353,18 +3344,18 @@
         <v>118</v>
       </c>
       <c r="L74" s="0" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="n">
         <v>7479194</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="D75" s="0" t="s">
         <v>74</v>
@@ -3373,7 +3364,7 @@
         <v>4</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="G75" s="0" t="s">
         <v>114</v>
@@ -3391,18 +3382,18 @@
         <v>118</v>
       </c>
       <c r="L75" s="0" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="n">
         <v>18422462</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D76" s="0" t="s">
         <v>74</v>
@@ -3411,7 +3402,7 @@
         <v>4</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G76" s="0" t="s">
         <v>114</v>
@@ -3429,18 +3420,18 @@
         <v>118</v>
       </c>
       <c r="L76" s="0" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="n">
         <v>19392810</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="D77" s="0" t="s">
         <v>74</v>
@@ -3449,7 +3440,7 @@
         <v>5</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G77" s="0" t="s">
         <v>114</v>
@@ -3467,18 +3458,18 @@
         <v>118</v>
       </c>
       <c r="L77" s="0" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="n">
         <v>19531695</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D78" s="0" t="s">
         <v>74</v>
@@ -3487,7 +3478,7 @@
         <v>4</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="G78" s="0" t="s">
         <v>114</v>
@@ -3505,18 +3496,18 @@
         <v>118</v>
       </c>
       <c r="L78" s="0" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="n">
         <v>19549709</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D79" s="0" t="s">
         <v>74</v>
@@ -3525,7 +3516,7 @@
         <v>4</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="G79" s="0" t="s">
         <v>114</v>
@@ -3543,7 +3534,7 @@
         <v>118</v>
       </c>
       <c r="L79" s="0" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3551,10 +3542,10 @@
         <v>20927253</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D80" s="0" t="s">
         <v>74</v>
@@ -3563,7 +3554,7 @@
         <v>5</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="G80" s="0" t="s">
         <v>114</v>
@@ -3572,7 +3563,7 @@
         <v>1</v>
       </c>
       <c r="I80" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J80" s="0" t="n">
         <v>0</v>
@@ -3581,7 +3572,7 @@
         <v>123</v>
       </c>
       <c r="L80" s="0" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3589,10 +3580,10 @@
         <v>24438483</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D81" s="0" t="s">
         <v>74</v>
@@ -3601,7 +3592,7 @@
         <v>4</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="G81" s="0" t="s">
         <v>114</v>
@@ -3619,7 +3610,7 @@
         <v>123</v>
       </c>
       <c r="L81" s="0" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3627,10 +3618,10 @@
         <v>24582773</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="D82" s="0" t="s">
         <v>74</v>
@@ -3639,7 +3630,7 @@
         <v>4</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="G82" s="0" t="s">
         <v>114</v>
@@ -3657,18 +3648,18 @@
         <v>123</v>
       </c>
       <c r="L82" s="0" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="n">
         <v>24733133</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="D83" s="0" t="s">
         <v>74</v>
@@ -3677,7 +3668,7 @@
         <v>4</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="G83" s="0" t="s">
         <v>114</v>
@@ -3695,18 +3686,18 @@
         <v>118</v>
       </c>
       <c r="L83" s="0" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="n">
         <v>24894748</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="D84" s="0" t="s">
         <v>74</v>
@@ -3715,7 +3706,7 @@
         <v>4</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="G84" s="0" t="s">
         <v>114</v>
@@ -3733,7 +3724,7 @@
         <v>118</v>
       </c>
       <c r="L84" s="0" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3741,10 +3732,10 @@
         <v>25907210</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="D85" s="0" t="s">
         <v>74</v>
@@ -3753,7 +3744,7 @@
         <v>4</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="G85" s="0" t="s">
         <v>114</v>
@@ -3762,7 +3753,7 @@
         <v>1</v>
       </c>
       <c r="I85" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J85" s="0" t="n">
         <v>0</v>
@@ -3771,7 +3762,7 @@
         <v>123</v>
       </c>
       <c r="L85" s="0" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3779,22 +3770,22 @@
         <v>256433</v>
       </c>
       <c r="B86" s="0" t="s">
+        <v>236</v>
+      </c>
+      <c r="C86" s="0" t="s">
+        <v>237</v>
+      </c>
+      <c r="D86" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E86" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F86" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="G86" s="0" t="s">
         <v>239</v>
-      </c>
-      <c r="C86" s="0" t="s">
-        <v>240</v>
-      </c>
-      <c r="D86" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="E86" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F86" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="G86" s="0" t="s">
-        <v>242</v>
       </c>
       <c r="H86" s="0" t="n">
         <v>0</v>
@@ -3809,7 +3800,7 @@
         <v>115</v>
       </c>
       <c r="L86" s="0" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3817,7 +3808,7 @@
         <v>448423</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C87" s="0" t="s">
         <v>112</v>
@@ -3829,10 +3820,10 @@
         <v>1</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="G87" s="0" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="H87" s="0" t="n">
         <v>0</v>
@@ -3844,10 +3835,10 @@
         <v>1</v>
       </c>
       <c r="K87" s="0" t="s">
-        <v>118</v>
+        <v>243</v>
       </c>
       <c r="L87" s="0" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3855,7 +3846,7 @@
         <v>448423</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C88" s="0" t="s">
         <v>112</v>
@@ -3867,10 +3858,10 @@
         <v>1</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="G88" s="0" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="H88" s="0" t="n">
         <v>0</v>
@@ -3882,10 +3873,10 @@
         <v>1</v>
       </c>
       <c r="K88" s="0" t="s">
-        <v>118</v>
+        <v>243</v>
       </c>
       <c r="L88" s="0" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3893,7 +3884,7 @@
         <v>448423</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C89" s="0" t="s">
         <v>112</v>
@@ -3905,10 +3896,10 @@
         <v>1</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="G89" s="0" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="H89" s="0" t="n">
         <v>0</v>
@@ -3920,10 +3911,10 @@
         <v>1</v>
       </c>
       <c r="K89" s="0" t="s">
-        <v>118</v>
+        <v>243</v>
       </c>
       <c r="L89" s="0" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3931,22 +3922,22 @@
         <v>2553470</v>
       </c>
       <c r="B90" s="0" t="s">
+        <v>247</v>
+      </c>
+      <c r="C90" s="0" t="s">
+        <v>248</v>
+      </c>
+      <c r="D90" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E90" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F90" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="C90" s="0" t="s">
-        <v>250</v>
-      </c>
-      <c r="D90" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="E90" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F90" s="2" t="s">
-        <v>251</v>
-      </c>
       <c r="G90" s="0" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="H90" s="0" t="n">
         <v>0</v>
@@ -3961,7 +3952,7 @@
         <v>115</v>
       </c>
       <c r="L90" s="0" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3969,10 +3960,10 @@
         <v>2553470</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C91" s="0" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D91" s="0" t="s">
         <v>14</v>
@@ -3981,10 +3972,10 @@
         <v>1</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G91" s="0" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="H91" s="0" t="n">
         <v>0</v>
@@ -3999,7 +3990,7 @@
         <v>115</v>
       </c>
       <c r="L91" s="0" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4007,10 +3998,10 @@
         <v>2553470</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C92" s="0" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D92" s="0" t="s">
         <v>14</v>
@@ -4019,10 +4010,10 @@
         <v>1</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G92" s="0" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="H92" s="0" t="n">
         <v>0</v>
@@ -4037,7 +4028,7 @@
         <v>115</v>
       </c>
       <c r="L92" s="0" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4045,7 +4036,7 @@
         <v>3191389</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C93" s="0" t="s">
         <v>84</v>
@@ -4057,10 +4048,10 @@
         <v>0</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="G93" s="0" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="H93" s="0" t="n">
         <v>0</v>
@@ -4075,7 +4066,7 @@
         <v>115</v>
       </c>
       <c r="L93" s="0" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4086,7 +4077,7 @@
         <v>22</v>
       </c>
       <c r="C94" s="0" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D94" s="0" t="s">
         <v>14</v>
@@ -4095,10 +4086,10 @@
         <v>3</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="G94" s="0" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="H94" s="0" t="n">
         <v>1</v>
@@ -4113,7 +4104,7 @@
         <v>123</v>
       </c>
       <c r="L94" s="0" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4121,37 +4112,37 @@
         <v>3711722</v>
       </c>
       <c r="B95" s="0" t="s">
+        <v>258</v>
+      </c>
+      <c r="C95" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="D95" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E95" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F95" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="G95" s="0" t="s">
+        <v>239</v>
+      </c>
+      <c r="H95" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I95" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J95" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K95" s="0" t="s">
         <v>260</v>
       </c>
-      <c r="C95" s="0" t="s">
-        <v>174</v>
-      </c>
-      <c r="D95" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="E95" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F95" s="2" t="s">
+      <c r="L95" s="0" t="s">
         <v>261</v>
-      </c>
-      <c r="G95" s="0" t="s">
-        <v>242</v>
-      </c>
-      <c r="H95" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I95" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J95" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K95" s="0" t="s">
-        <v>262</v>
-      </c>
-      <c r="L95" s="0" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4159,7 +4150,7 @@
         <v>9061777</v>
       </c>
       <c r="B96" s="0" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C96" s="0" t="s">
         <v>84</v>
@@ -4171,10 +4162,10 @@
         <v>3</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="G96" s="0" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="H96" s="0" t="n">
         <v>1</v>
@@ -4189,7 +4180,7 @@
         <v>123</v>
       </c>
       <c r="L96" s="0" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4197,7 +4188,7 @@
         <v>9061777</v>
       </c>
       <c r="B97" s="0" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C97" s="0" t="s">
         <v>84</v>
@@ -4209,10 +4200,10 @@
         <v>3</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="G97" s="0" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="H97" s="0" t="n">
         <v>1</v>
@@ -4227,7 +4218,7 @@
         <v>123</v>
       </c>
       <c r="L97" s="0" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4235,7 +4226,7 @@
         <v>9061777</v>
       </c>
       <c r="B98" s="0" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C98" s="0" t="s">
         <v>84</v>
@@ -4247,10 +4238,10 @@
         <v>3</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="G98" s="0" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="H98" s="0" t="n">
         <v>1</v>
@@ -4265,7 +4256,7 @@
         <v>123</v>
       </c>
       <c r="L98" s="0" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4273,7 +4264,7 @@
         <v>9061777</v>
       </c>
       <c r="B99" s="0" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C99" s="0" t="s">
         <v>84</v>
@@ -4285,10 +4276,10 @@
         <v>3</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="G99" s="0" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="H99" s="0" t="n">
         <v>1</v>
@@ -4303,7 +4294,7 @@
         <v>123</v>
       </c>
       <c r="L99" s="0" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4311,7 +4302,7 @@
         <v>10427794</v>
       </c>
       <c r="B100" s="0" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C100" s="0" t="s">
         <v>126</v>
@@ -4323,13 +4314,13 @@
         <v>1</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G100" s="0" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="H100" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I100" s="0" t="n">
         <v>1</v>
@@ -4341,7 +4332,7 @@
         <v>115</v>
       </c>
       <c r="L100" s="0" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4349,22 +4340,22 @@
         <v>16906379</v>
       </c>
       <c r="B101" s="0" t="s">
+        <v>271</v>
+      </c>
+      <c r="C101" s="0" t="s">
+        <v>272</v>
+      </c>
+      <c r="D101" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E101" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F101" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="C101" s="0" t="s">
-        <v>274</v>
-      </c>
-      <c r="D101" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="E101" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F101" s="2" t="s">
-        <v>275</v>
-      </c>
       <c r="G101" s="0" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="H101" s="0" t="n">
         <v>0</v>
@@ -4379,7 +4370,7 @@
         <v>115</v>
       </c>
       <c r="L101" s="0" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4387,22 +4378,22 @@
         <v>20447294</v>
       </c>
       <c r="B102" s="0" t="s">
+        <v>275</v>
+      </c>
+      <c r="C102" s="0" t="s">
+        <v>276</v>
+      </c>
+      <c r="D102" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E102" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F102" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="C102" s="0" t="s">
-        <v>278</v>
-      </c>
-      <c r="D102" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="E102" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F102" s="2" t="s">
-        <v>279</v>
-      </c>
       <c r="G102" s="0" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="H102" s="0" t="n">
         <v>0</v>
@@ -4417,7 +4408,7 @@
         <v>115</v>
       </c>
       <c r="L102" s="0" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4425,10 +4416,10 @@
         <v>23433219</v>
       </c>
       <c r="B103" s="0" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C103" s="0" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D103" s="0" t="s">
         <v>14</v>
@@ -4437,10 +4428,10 @@
         <v>3</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="G103" s="0" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="H103" s="0" t="n">
         <v>0</v>
@@ -4455,7 +4446,7 @@
         <v>115</v>
       </c>
       <c r="L103" s="0" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4463,10 +4454,10 @@
         <v>24665854</v>
       </c>
       <c r="B104" s="0" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C104" s="0" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D104" s="0" t="s">
         <v>14</v>
@@ -4475,25 +4466,25 @@
         <v>3</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="G104" s="0" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="H104" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I104" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J104" s="0" t="n">
         <v>0</v>
       </c>
       <c r="K104" s="0" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="L104" s="0" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4501,37 +4492,37 @@
         <v>24733133</v>
       </c>
       <c r="B105" s="0" t="s">
+        <v>287</v>
+      </c>
+      <c r="C105" s="0" t="s">
+        <v>288</v>
+      </c>
+      <c r="D105" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E105" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F105" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="C105" s="0" t="s">
+      <c r="G105" s="0" t="s">
+        <v>239</v>
+      </c>
+      <c r="H105" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I105" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J105" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K105" s="0" t="s">
+        <v>243</v>
+      </c>
+      <c r="L105" s="0" t="s">
         <v>290</v>
-      </c>
-      <c r="D105" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="E105" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F105" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="G105" s="0" t="s">
-        <v>242</v>
-      </c>
-      <c r="H105" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I105" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="J105" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K105" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="L105" s="0" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4539,10 +4530,10 @@
         <v>24840785</v>
       </c>
       <c r="B106" s="0" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C106" s="0" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D106" s="0" t="s">
         <v>14</v>
@@ -4551,25 +4542,25 @@
         <v>2</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="G106" s="0" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="H106" s="0" t="n">
         <v>1</v>
       </c>
       <c r="I106" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J106" s="0" t="n">
         <v>0</v>
       </c>
       <c r="K106" s="0" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="L106" s="0" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4577,10 +4568,10 @@
         <v>24927617</v>
       </c>
       <c r="B107" s="0" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C107" s="0" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D107" s="0" t="s">
         <v>14</v>
@@ -4589,10 +4580,10 @@
         <v>2</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="G107" s="0" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="H107" s="0" t="n">
         <v>0</v>
@@ -4607,7 +4598,7 @@
         <v>115</v>
       </c>
       <c r="L107" s="0" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4615,7 +4606,7 @@
         <v>1779253</v>
       </c>
       <c r="B108" s="0" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C108" s="0" t="s">
         <v>73</v>
@@ -4627,10 +4618,10 @@
         <v>1</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="G108" s="0" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="H108" s="0" t="n">
         <v>0</v>
@@ -4642,10 +4633,10 @@
         <v>1</v>
       </c>
       <c r="K108" s="0" t="s">
-        <v>118</v>
+        <v>243</v>
       </c>
       <c r="L108" s="0" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4653,7 +4644,7 @@
         <v>6106951</v>
       </c>
       <c r="B109" s="0" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C109" s="0" t="s">
         <v>84</v>
@@ -4665,10 +4656,10 @@
         <v>1</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="G109" s="0" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="H109" s="0" t="n">
         <v>1</v>
@@ -4683,18 +4674,18 @@
         <v>123</v>
       </c>
       <c r="L109" s="0" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="n">
         <v>8667442</v>
       </c>
       <c r="B110" s="0" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C110" s="0" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D110" s="0" t="s">
         <v>74</v>
@@ -4703,10 +4694,10 @@
         <v>1</v>
       </c>
       <c r="F110" s="2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="G110" s="0" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="H110" s="0" t="n">
         <v>0</v>
@@ -4718,10 +4709,10 @@
         <v>1</v>
       </c>
       <c r="K110" s="0" t="s">
-        <v>118</v>
+        <v>243</v>
       </c>
       <c r="L110" s="0" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4741,10 +4732,10 @@
         <v>2</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="G111" s="0" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="H111" s="0" t="n">
         <v>1</v>
@@ -4759,7 +4750,7 @@
         <v>123</v>
       </c>
       <c r="L111" s="0" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4767,7 +4758,7 @@
         <v>9071336</v>
       </c>
       <c r="B112" s="0" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C112" s="0" t="s">
         <v>107</v>
@@ -4779,10 +4770,10 @@
         <v>3</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G112" s="0" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="H112" s="0" t="n">
         <v>1</v>
@@ -4797,18 +4788,18 @@
         <v>123</v>
       </c>
       <c r="L112" s="0" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="n">
         <v>9428298</v>
       </c>
       <c r="B113" s="0" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C113" s="0" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D113" s="0" t="s">
         <v>74</v>
@@ -4817,10 +4808,10 @@
         <v>2</v>
       </c>
       <c r="F113" s="2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="G113" s="0" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="H113" s="0" t="n">
         <v>0</v>
@@ -4832,21 +4823,21 @@
         <v>0</v>
       </c>
       <c r="K113" s="0" t="s">
-        <v>316</v>
+        <v>260</v>
       </c>
       <c r="L113" s="0" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="n">
         <v>9578276</v>
       </c>
       <c r="B114" s="0" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="C114" s="0" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="D114" s="0" t="s">
         <v>74</v>
@@ -4855,10 +4846,10 @@
         <v>3</v>
       </c>
       <c r="F114" s="2" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="G114" s="0" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="H114" s="0" t="n">
         <v>0</v>
@@ -4870,10 +4861,10 @@
         <v>1</v>
       </c>
       <c r="K114" s="0" t="s">
-        <v>118</v>
+        <v>243</v>
       </c>
       <c r="L114" s="0" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4881,10 +4872,10 @@
         <v>11745287</v>
       </c>
       <c r="B115" s="0" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="C115" s="0" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="D115" s="0" t="s">
         <v>74</v>
@@ -4893,10 +4884,10 @@
         <v>2</v>
       </c>
       <c r="F115" s="2" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="G115" s="0" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="H115" s="0" t="n">
         <v>1</v>
@@ -4911,7 +4902,7 @@
         <v>123</v>
       </c>
       <c r="L115" s="0" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4922,7 +4913,7 @@
         <v>88</v>
       </c>
       <c r="C116" s="0" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="D116" s="0" t="s">
         <v>74</v>
@@ -4931,10 +4922,10 @@
         <v>3</v>
       </c>
       <c r="F116" s="2" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="G116" s="0" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="H116" s="0" t="n">
         <v>1</v>
@@ -4949,7 +4940,7 @@
         <v>123</v>
       </c>
       <c r="L116" s="0" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4957,7 +4948,7 @@
         <v>17223814</v>
       </c>
       <c r="B117" s="0" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="C117" s="0" t="s">
         <v>27</v>
@@ -4969,10 +4960,10 @@
         <v>1</v>
       </c>
       <c r="F117" s="2" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="G117" s="0" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="H117" s="0" t="n">
         <v>1</v>
@@ -4987,7 +4978,7 @@
         <v>123</v>
       </c>
       <c r="L117" s="0" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4998,7 +4989,7 @@
         <v>94</v>
       </c>
       <c r="C118" s="0" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="D118" s="0" t="s">
         <v>74</v>
@@ -5007,10 +4998,10 @@
         <v>3</v>
       </c>
       <c r="F118" s="2" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="G118" s="0" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="H118" s="0" t="n">
         <v>1</v>
@@ -5025,7 +5016,7 @@
         <v>123</v>
       </c>
       <c r="L118" s="0" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5033,10 +5024,10 @@
         <v>17356399</v>
       </c>
       <c r="B119" s="0" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="C119" s="0" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="D119" s="0" t="s">
         <v>74</v>
@@ -5045,10 +5036,10 @@
         <v>3</v>
       </c>
       <c r="F119" s="2" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="G119" s="0" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="H119" s="0" t="n">
         <v>1</v>
@@ -5063,15 +5054,15 @@
         <v>123</v>
       </c>
       <c r="L119" s="0" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="n">
         <v>18987260</v>
       </c>
       <c r="B120" s="0" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C120" s="0" t="s">
         <v>64</v>
@@ -5083,10 +5074,10 @@
         <v>2</v>
       </c>
       <c r="F120" s="2" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="G120" s="0" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="H120" s="0" t="n">
         <v>0</v>
@@ -5098,10 +5089,10 @@
         <v>0</v>
       </c>
       <c r="K120" s="0" t="s">
-        <v>316</v>
+        <v>260</v>
       </c>
       <c r="L120" s="0" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5109,10 +5100,10 @@
         <v>19139825</v>
       </c>
       <c r="B121" s="0" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C121" s="0" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="D121" s="0" t="s">
         <v>74</v>
@@ -5121,10 +5112,10 @@
         <v>3</v>
       </c>
       <c r="F121" s="2" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="G121" s="0" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="H121" s="0" t="n">
         <v>1</v>
@@ -5139,7 +5130,7 @@
         <v>123</v>
       </c>
       <c r="L121" s="0" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5147,10 +5138,10 @@
         <v>19549709</v>
       </c>
       <c r="B122" s="0" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C122" s="0" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="D122" s="0" t="s">
         <v>74</v>
@@ -5159,10 +5150,10 @@
         <v>3</v>
       </c>
       <c r="F122" s="2" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="G122" s="0" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="H122" s="0" t="n">
         <v>1</v>
@@ -5177,7 +5168,7 @@
         <v>123</v>
       </c>
       <c r="L122" s="0" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix comment parity for crowd error analysis.
Propagated Ben's comments to multiple tasks for the same relation.
</commit_message>
<xml_diff>
--- a/crowd_only/data/final_eval/analysis/crowd_testset_perfect_ner_errors.xlsx
+++ b/crowd_only/data/final_eval/analysis/crowd_testset_perfect_ner_errors.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="340">
   <si>
     <t>pmid</t>
   </si>
@@ -632,6 +632,9 @@
     <t>if anything it’s a "treats" relationship</t>
   </si>
   <si>
+    <t>these I think are examples where sentence scoping hurts</t>
+  </si>
+  <si>
     <t>Text never says that EACA causes SAH. If anything, it only says that EACA is good for treating rebleeding for patients with SAH.</t>
   </si>
   <si>
@@ -639,9 +642,6 @@
   </si>
   <si>
     <t>https://crowdflower.com/jobs/767262/units/773932444</t>
-  </si>
-  <si>
-    <t>these I think are examples where sentence scoping hurts</t>
   </si>
   <si>
     <t>MESH:D008094</t>
@@ -1166,7 +1166,7 @@
   <dimension ref="A1:S78"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S32" activeCellId="0" sqref="S32"/>
+      <selection pane="topLeft" activeCell="Q25" activeCellId="0" sqref="Q25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2436,6 +2436,9 @@
       <c r="P25" s="0" t="s">
         <v>49</v>
       </c>
+      <c r="Q25" s="0" t="s">
+        <v>107</v>
+      </c>
       <c r="S25" s="0" t="s">
         <v>108</v>
       </c>
@@ -3384,8 +3387,11 @@
       <c r="Q43" s="0" t="s">
         <v>204</v>
       </c>
+      <c r="R43" s="0" t="s">
+        <v>205</v>
+      </c>
       <c r="S43" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3408,7 +3414,7 @@
         <v>22</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="H44" s="0" t="s">
         <v>199</v>
@@ -3437,8 +3443,14 @@
       <c r="P44" s="0" t="s">
         <v>203</v>
       </c>
+      <c r="Q44" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="R44" s="0" t="s">
+        <v>205</v>
+      </c>
       <c r="S44" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3461,7 +3473,7 @@
         <v>22</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="H45" s="0" t="s">
         <v>199</v>
@@ -3490,11 +3502,14 @@
       <c r="P45" s="0" t="s">
         <v>203</v>
       </c>
+      <c r="Q45" s="0" t="s">
+        <v>204</v>
+      </c>
       <c r="R45" s="0" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="S45" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Fix label of one error as a task limitation.
Fixed annotating one crowd error as a task limitation.
</commit_message>
<xml_diff>
--- a/crowd_only/data/final_eval/analysis/crowd_testset_perfect_ner_errors.xlsx
+++ b/crowd_only/data/final_eval/analysis/crowd_testset_perfect_ner_errors.xlsx
@@ -1165,8 +1165,8 @@
   </sheetPr>
   <dimension ref="A1:S78"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q25" activeCellId="0" sqref="Q25"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q62" activeCellId="0" sqref="Q62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -4314,7 +4314,7 @@
         <v>0</v>
       </c>
       <c r="P62" s="0" t="s">
-        <v>227</v>
+        <v>31</v>
       </c>
       <c r="S62" s="0" t="s">
         <v>267</v>

</xml_diff>